<commit_message>
revisi Laporan Sesuai Sisdur Tahap 1
</commit_message>
<xml_diff>
--- a/utility/optbs/template/bukti_pengambilan_barang.xlsx
+++ b/utility/optbs/template/bukti_pengambilan_barang.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>SKPD</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>Pekalongan,      Tahun</t>
+  </si>
+  <si>
+    <t>Mengetahui</t>
+  </si>
+  <si>
+    <t>Yang Menerima</t>
+  </si>
+  <si>
+    <t>Yang Menyerahkan</t>
+  </si>
+  <si>
+    <t>……………………………………..</t>
+  </si>
+  <si>
+    <t>NIP…………………………….</t>
   </si>
 </sst>
 </file>
@@ -117,8 +132,8 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Bookman Old Style"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -205,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +229,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +267,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -327,181 +354,218 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="11.0714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>